<commit_message>
random Global ID generator
</commit_message>
<xml_diff>
--- a/routes/Data/MJTdata_projectlist1.xlsx
+++ b/routes/Data/MJTdata_projectlist1.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -46,7 +46,7 @@
     <t>ProjectDesc#string</t>
   </si>
   <si>
-    <t xml:space="preserve">GlobalID: MJT001; inProjectID: WMA01, GlobalID: MJT002; inProjectID: WMA02,GlobalID: MJT003; inProjectID: WMA04, GlobalID: MJT004; inProjectID: WMA04, GlobalID: MJT005; inProjectID: WMA05 </t>
+    <t xml:space="preserve">GlobalID: MJT001; inProjectID: WMA01, GlobalID: MJT002; inProjectID: WMA02, GlobalID: MJT003; inProjectID: WMA04, GlobalID: MJT004; inProjectID: WMA04, GlobalID: MJT005; inProjectID: WMA05 </t>
   </si>
 </sst>
 </file>
@@ -82,8 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +394,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +403,7 @@
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -423,7 +426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -436,11 +439,12 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>